<commit_message>
feat: improve code readability, navigation, and section ordering
</commit_message>
<xml_diff>
--- a/docs/source/docs.xlsx
+++ b/docs/source/docs.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\git\DocForge\docs\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2791171B-C558-4733-AB55-B459D28B983E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDC76B6-45FF-4766-8FFA-3990C600458F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37170" yWindow="3210" windowWidth="26490" windowHeight="18390" xr2:uid="{36479354-C0A0-4D04-A6BB-51F46C906E37}"/>
+    <workbookView xWindow="-29175" yWindow="8760" windowWidth="28800" windowHeight="18015" xr2:uid="{36479354-C0A0-4D04-A6BB-51F46C906E37}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
+    <sheet name="Meta" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Content!$A$1:$I$1</definedName>
+    <definedName name="BoolList">Meta!$D$3:$D$4</definedName>
+    <definedName name="LangList">Meta!$C$3:$C$12</definedName>
+    <definedName name="TypeList">Meta!$B$3:$B$12</definedName>
+  </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="48">
   <si>
     <t>Chapter</t>
   </si>
@@ -62,37 +69,149 @@
     <t xml:space="preserve">Git </t>
   </si>
   <si>
-    <t xml:space="preserve"> Init → First push </t>
-  </si>
-  <si>
     <t xml:space="preserve"> text </t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> Erklärung... </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PowerShell </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Profil laden </t>
-  </si>
-  <si>
     <t xml:space="preserve"> code </t>
   </si>
   <si>
-    <t xml:space="preserve"> powershell </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> . $PROFILE </t>
-  </si>
-  <si>
     <t xml:space="preserve"> true</t>
+  </si>
+  <si>
+    <t>Clone into a new repository (without history)</t>
+  </si>
+  <si>
+    <t>Sometimes you want to reuse a repository as a starting point, but keep a completely clean history.</t>
+  </si>
+  <si>
+    <t>ChapterOrder</t>
+  </si>
+  <si>
+    <t>SectionOrder</t>
+  </si>
+  <si>
+    <t>bash</t>
+  </si>
+  <si>
+    <t>git clone https://github.com/original/project.git
+cd project
+rm -rf .git
+git init
+git remote add origin https://github.com/you/new-repo.git
+git add .
+git commit -m "Initial commit"
+git push -u origin main</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Removing .git also removes the original remote.
+You must explicitly configure a new one before pushing.</t>
+  </si>
+  <si>
+    <t>TypeList</t>
+  </si>
+  <si>
+    <t>LangList</t>
+  </si>
+  <si>
+    <t>BoolList</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>powershell</t>
+  </si>
+  <si>
+    <t>markup</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>First commit and push to a new repository</t>
+  </si>
+  <si>
+    <t>After creating a new repository (for example on GitHub), the first commit establishes the initial project state and connects it to the remote.</t>
+  </si>
+  <si>
+    <t>git init
+git add .
+git commit -m "Initial commit"
+git remote add origin https://github.com/you/project.git
+git push -u origin main</t>
+  </si>
+  <si>
+    <t>The -u flag sets the upstream branch, allowing future git push
+and git pull commands without specifying the remote.</t>
+  </si>
+  <si>
+    <t>Separate feature and documentation commits</t>
+  </si>
+  <si>
+    <t>Keeping functional changes and documentation updates in separate commits
+improves readability and makes code reviews easier.</t>
+  </si>
+  <si>
+    <t>git restore --staged README.md
+git add build/build-docs.ps1
+git commit -m "feat(build): add multi-workbook support"</t>
+  </si>
+  <si>
+    <t>This approach makes the intent of each commit explicit
+and results in a cleaner project history.</t>
+  </si>
+  <si>
+    <t>Create and push a release tag</t>
+  </si>
+  <si>
+    <t>Tags are commonly used to mark release points in the repository history.
+They can also be created after the fact.</t>
+  </si>
+  <si>
+    <t>Tags are lightweight references and do not modify the commit history.
+Creating them later is perfectly fine.</t>
+  </si>
+  <si>
+    <t>git tag v0.6.0
+git push --tags</t>
+  </si>
+  <si>
+    <t>git add .
+git restore --staged README.md</t>
+  </si>
+  <si>
+    <t>git status
+git diff --staged</t>
+  </si>
+  <si>
+    <t>git commit -m "feat(build): add multi-workbook support"
+git add README.md
+git commit -m "docs: update README for v0.6.0"</t>
+  </si>
+  <si>
+    <t>Mulitple feature and documentation commits</t>
+  </si>
+  <si>
+    <t>Keeping multiple functional changes and documentation update in separate commits
+improves readability and makes code reviews easier.</t>
+  </si>
+  <si>
+    <t>Check status of staged files</t>
   </si>
 </sst>
 </file>
@@ -108,15 +227,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -124,12 +249,236 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -464,113 +813,1049 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8011AD-E0FB-4176-ADB9-7ED8BA29C820}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="19.86328125" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
-    <col min="6" max="6" width="24.265625" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="1" max="1" width="23.59765625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.59765625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="10.6640625" style="2"/>
+    <col min="7" max="7" width="18" style="2" customWidth="1"/>
+    <col min="8" max="8" width="56.3984375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.9296875" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="13">
+        <v>10</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="13">
+        <v>10</v>
+      </c>
+      <c r="E2" s="13">
+        <v>10</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="G2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="128.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E3" s="6">
+        <v>20</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="19">
+        <v>10</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3">
+      <c r="D4" s="19">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E4" s="19">
+        <v>30</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="13">
+        <v>20</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="13">
+        <v>20</v>
+      </c>
+      <c r="E5" s="13">
+        <v>10</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="6">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6">
+        <v>20</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="19">
+        <v>20</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="19">
+        <v>20</v>
+      </c>
+      <c r="E7" s="19">
+        <v>30</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
+      <c r="G7" s="19"/>
+      <c r="H7" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13">
+        <v>30</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="13">
+        <v>30</v>
+      </c>
+      <c r="E8" s="13">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6">
+        <v>30</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="6">
+        <v>30</v>
+      </c>
+      <c r="E9" s="6">
+        <v>20</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="19">
+        <v>30</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="19">
+        <v>30</v>
+      </c>
+      <c r="E10" s="19">
+        <v>70</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="13">
+        <v>32</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="13">
+        <v>32</v>
+      </c>
+      <c r="E11" s="13">
+        <v>10</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="6">
+        <v>32</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="6">
+        <v>32</v>
+      </c>
+      <c r="E12" s="6">
+        <v>40</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="6">
+        <v>32</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="6">
+        <v>32</v>
+      </c>
+      <c r="E13" s="6">
+        <v>40</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6">
+        <v>32</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="6">
+        <v>32</v>
+      </c>
+      <c r="E14" s="6">
+        <v>50</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6">
+        <v>32</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="6">
+        <v>32</v>
+      </c>
+      <c r="E15" s="6">
+        <v>60</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="19">
+        <v>32</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="19">
+        <v>32</v>
+      </c>
+      <c r="E16" s="19">
+        <v>70</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="13">
+        <v>40</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="13">
+        <v>40</v>
+      </c>
+      <c r="E17" s="13">
+        <v>10</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="6">
+        <v>40</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="6">
+        <v>40</v>
+      </c>
+      <c r="E18" s="6">
+        <v>20</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="19">
+        <v>40</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="19">
+        <v>40</v>
+      </c>
+      <c r="E19" s="19">
+        <v>30</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="6"/>
+    </row>
+    <row r="50" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="6"/>
+    </row>
+    <row r="51" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="6"/>
+    </row>
+    <row r="52" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="6"/>
+    </row>
+    <row r="53" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="6"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{3C8011AD-E0FB-4176-ADB9-7ED8BA29C820}"/>
+  <dataConsolidate/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6 G18 F1:F1048576" xr:uid="{F8E8FCAB-C278-48F1-9D6C-445863CE5337}">
+      <formula1>TypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G5 G19:G1048576 G7:G17" xr:uid="{AEDB114F-DF78-4BAF-AA24-46550AFA1A05}">
+      <formula1>LangList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{EF6ED930-73E6-4830-95C1-3A9D0AB6ECD0}">
+      <formula1>BoolList</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51DFB226-5908-4826-B203-387F1FE00B61}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="20" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="3.59765625" style="3" customWidth="1"/>
+    <col min="2" max="4" width="15.59765625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="3.59765625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.6640625" style="3" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="2:4" ht="20" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>